<commit_message>
webrework work in process : cdn file move locally : what size ?
</commit_message>
<xml_diff>
--- a/_3_software/IoT_EPS/dataSavDir/fileListe220820_2144.xlsx
+++ b/_3_software/IoT_EPS/dataSavDir/fileListe220820_2144.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojo\Documents\jojoBag\perso\0044-Iot_ESP_PPlug\projet\_3_software\IoT_EPS\dataSavDir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E0FC114-47EB-49B9-AA67-DCABF729AF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DE029904-7F8E-4E60-8090-D93D8E43AA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fileListe220820_2144" sheetId="1" r:id="rId1"/>
+    <sheet name="fileListe220903_1701" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="97" uniqueCount="44">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="155" uniqueCount="54">
   <si>
     <t xml:space="preserve">apmodeindex.htm </t>
   </si>
@@ -157,12 +169,42 @@
   </si>
   <si>
     <t>SPIFFS max path lenght : 32</t>
+  </si>
+  <si>
+    <t>220820_2147</t>
+  </si>
+  <si>
+    <t>fileListe220820_2144</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>SPIFFS used bytes : 603404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jquery-3.3.1.min.js </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bootstrap.min.js </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bootstrap.min.css </t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -299,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,8 +521,26 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <start/>
       <end/>
@@ -595,6 +655,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="medium">
+        <color indexed="64"/>
+      </start>
+      <end/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <start/>
+      <end style="medium">
+        <color indexed="64"/>
+      </end>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -640,8 +737,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -996,568 +1107,901 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="11" max="11" width="2.28515625" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="D3">
         <v>1303</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="J1">
+      <c r="J3">
         <v>1303</v>
       </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="P3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>3405</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I4" t="s">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="J4">
         <v>3405</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>11966</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D5">
         <v>3279</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="J5">
         <v>3279</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>170</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="J6">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1074</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>2021</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>3738</v>
+        <v>1074</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
       </c>
       <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>1074</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8">
+        <v>140942</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>2021</v>
+      </c>
+      <c r="O9" t="s">
+        <v>4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="J7">
+      <c r="D10">
         <v>3738</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>3738</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>5183</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>1407</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I11" t="s">
         <v>8</v>
       </c>
-      <c r="J8">
+      <c r="J11">
         <v>1407</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="P11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <v>7890</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <v>5384</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I13" t="s">
         <v>10</v>
       </c>
-      <c r="J10">
+      <c r="J13">
         <v>5384</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="P13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13">
+        <v>7053</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D11">
+      <c r="D14">
         <v>5289</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="D12">
+      <c r="D15">
         <v>1275</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I15" t="s">
         <v>12</v>
       </c>
-      <c r="J12">
+      <c r="J15">
         <v>1275</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="P15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>1246</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I16" t="s">
         <v>14</v>
       </c>
-      <c r="J13">
+      <c r="J16">
         <v>722</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="L16">
+        <f>D16-J16</f>
+        <v>524</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-      <c r="D14">
+      <c r="D17">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16">
-        <v>12473</v>
-      </c>
-      <c r="H16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16">
-        <v>12473</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>27773</v>
-      </c>
-      <c r="H17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17">
-        <v>13317</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D18">
-        <v>32887</v>
-      </c>
-      <c r="H18" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18">
-        <v>32887</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D19">
-        <v>28171</v>
+        <v>12473</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J19">
-        <v>12775</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+        <v>12473</v>
+      </c>
+      <c r="O19" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19">
+        <v>28607</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>30460</v>
+        <v>27773</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
       </c>
       <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20">
+        <v>13317</v>
+      </c>
+      <c r="O20" t="s">
+        <v>16</v>
+      </c>
+      <c r="P20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20">
+        <v>27773</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>32887</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21">
+        <v>32887</v>
+      </c>
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q21">
+        <v>84044</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>28171</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22">
+        <v>12775</v>
+      </c>
+      <c r="O22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22">
+        <v>28171</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="J20">
+      <c r="D23">
+        <v>30460</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23">
         <v>15965</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="O23" t="s">
+        <v>16</v>
+      </c>
+      <c r="P23" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23">
+        <v>30460</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>48741</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I24" t="s">
         <v>24</v>
       </c>
-      <c r="J21">
+      <c r="J24">
         <v>5051</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="L24">
+        <f>D24-J24</f>
+        <v>43690</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q24">
+        <v>4952</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>25</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>16109</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I25" t="s">
         <v>25</v>
       </c>
-      <c r="J22">
+      <c r="J25">
         <v>16109</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
+      <c r="P26" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q26">
+        <v>51045</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27">
+        <v>86929</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="D23">
+      <c r="D28">
         <v>13904</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H28" t="s">
         <v>26</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I28" t="s">
         <v>27</v>
       </c>
-      <c r="J23">
+      <c r="J28">
         <v>13904</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="O28" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="P28" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28">
+        <v>14770</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="D24">
+      <c r="D29">
         <v>712</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H29" t="s">
         <v>26</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I29" t="s">
         <v>28</v>
       </c>
-      <c r="J24">
+      <c r="J29">
         <v>712</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="O29" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
+      <c r="P29" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q29">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>26</v>
+      </c>
+      <c r="P30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D25">
+      <c r="Q30">
+        <v>18462</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
         <v>18959</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H31" t="s">
         <v>26</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I31" t="s">
         <v>30</v>
       </c>
-      <c r="J25">
+      <c r="J31">
         <v>3120</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="L31">
+        <f>D31-J31</f>
+        <v>15839</v>
+      </c>
+      <c r="O31" t="s">
         <v>26</v>
       </c>
-      <c r="C26" t="s">
+      <c r="P31" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q31">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="D26">
+      <c r="D32">
         <v>8724</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H32" t="s">
         <v>26</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I32" t="s">
         <v>31</v>
       </c>
-      <c r="J26">
+      <c r="J32">
         <v>8724</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="O32" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
+      <c r="P32" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q32">
+        <v>8724</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="D27">
+      <c r="D33">
         <v>8425</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H33" t="s">
         <v>26</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I33" t="s">
         <v>32</v>
       </c>
-      <c r="J27">
+      <c r="J33">
         <v>8425</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="O33" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q33">
+        <v>8737</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="D28">
+      <c r="D34">
         <v>1380</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I34" t="s">
         <v>33</v>
       </c>
-      <c r="J28">
+      <c r="J34">
         <v>1380</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="P34" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q34">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="D29">
+      <c r="D35">
         <v>12531</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I35" t="s">
         <v>34</v>
       </c>
-      <c r="J29">
+      <c r="J35">
         <v>12531</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="P35" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q35">
+        <v>12531</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D30">
+      <c r="D36">
         <v>198</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I36" t="s">
         <v>35</v>
       </c>
-      <c r="J30">
+      <c r="J36">
         <v>198</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="P36" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q36">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D31">
+      <c r="D37">
         <v>1408</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I37" t="s">
         <v>37</v>
       </c>
-      <c r="J31">
+      <c r="J37">
         <v>1408</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="P37" t="s">
         <v>37</v>
       </c>
-      <c r="D32">
+      <c r="Q37">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
         <v>1419</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I38" t="s">
         <v>38</v>
       </c>
-      <c r="J32">
+      <c r="J38">
         <v>1408</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="P38" t="s">
         <v>38</v>
       </c>
-      <c r="D33">
+      <c r="Q38">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39">
         <v>1419</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I39" t="s">
         <v>36</v>
       </c>
-      <c r="J33">
+      <c r="J39">
         <v>1408</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="P39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q39">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="D34">
+      <c r="D40">
         <v>303875</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="J40">
+        <f>SUM(J3:J39)</f>
+        <v>185573</v>
+      </c>
+      <c r="N40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q40">
+        <f>SUM(Q3:Q39)</f>
+        <v>587973</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="N41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="N42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G43" t="s">
         <v>43</v>
       </c>
+      <c r="N43" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37123C97-52BA-4579-9B37-3D1077B298A2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lots of documentation works
</commit_message>
<xml_diff>
--- a/_3_software/IoT_EPS/dataSavDir/fileListe220820_2144.xlsx
+++ b/_3_software/IoT_EPS/dataSavDir/fileListe220820_2144.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jojo\Documents\jojoBag\perso\0044-Iot_ESP_PPlug\projet\_3_software\IoT_EPS\dataSavDir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DE029904-7F8E-4E60-8090-D93D8E43AA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AD80E6AB-754B-405C-927C-D721CA43F5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="155" uniqueCount="54">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="161" uniqueCount="60">
   <si>
     <t xml:space="preserve">apmodeindex.htm </t>
   </si>
@@ -180,9 +180,6 @@
     <t>delta</t>
   </si>
   <si>
-    <t>SPIFFS used bytes : 603404</t>
-  </si>
-  <si>
     <t xml:space="preserve">jquery-3.3.1.min.js </t>
   </si>
   <si>
@@ -199,6 +196,27 @@
   </si>
   <si>
     <t>size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPIFFS used bytes : </t>
+  </si>
+  <si>
+    <t>reste</t>
+  </si>
+  <si>
+    <t>- js/jquery-ui.1.12.1.min.js</t>
+  </si>
+  <si>
+    <t>- js/solid.5.0.13.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- js/fontawesome.5.0.13.js </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- js/popper.1.14.6.min.js </t>
+  </si>
+  <si>
+    <t>220903_1701</t>
   </si>
 </sst>
 </file>
@@ -341,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +554,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,8 +761,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -748,11 +774,10 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1108,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,32 +1148,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="H1" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="H1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="5"/>
       <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="O1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
         <v>51</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -1255,13 +1282,13 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O8" t="s">
+      <c r="O8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="P8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8">
+      <c r="P8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="7">
         <v>140942</v>
       </c>
     </row>
@@ -1416,7 +1443,7 @@
         <f>D16-J16</f>
         <v>524</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="P16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Q16">
@@ -1604,7 +1631,7 @@
         <f>D24-J24</f>
         <v>43690</v>
       </c>
-      <c r="P24" s="4" t="s">
+      <c r="P24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="Q24">
@@ -1626,24 +1653,24 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O26" t="s">
+      <c r="O26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P26" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q26">
+      <c r="P26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="7">
         <v>51045</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="O27" t="s">
+      <c r="O27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P27" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q27">
+      <c r="P27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q27" s="7">
         <v>86929</v>
       </c>
     </row>
@@ -1709,7 +1736,7 @@
       <c r="O30" t="s">
         <v>26</v>
       </c>
-      <c r="P30" s="5" t="s">
+      <c r="P30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q30">
@@ -1944,6 +1971,9 @@
       <c r="N40" t="s">
         <v>39</v>
       </c>
+      <c r="P40">
+        <v>2949250</v>
+      </c>
       <c r="Q40">
         <f>SUM(Q3:Q39)</f>
         <v>587973</v>
@@ -1957,7 +1987,10 @@
         <v>41</v>
       </c>
       <c r="N41" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="P41">
+        <v>603404</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -1970,6 +2003,13 @@
       <c r="N42" t="s">
         <v>42</v>
       </c>
+      <c r="P42" s="6">
+        <f>P40-P41</f>
+        <v>2345846</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1980,6 +2020,54 @@
       </c>
       <c r="N43" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q46" s="9">
+        <f>248*1024</f>
+        <v>253952</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N47" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q47">
+        <f>343*1024</f>
+        <v>351232</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N48" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q48">
+        <f>27*1024</f>
+        <v>27648</v>
+      </c>
+    </row>
+    <row r="49" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="N49" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q49">
+        <f>22*1024</f>
+        <v>22528</v>
+      </c>
+    </row>
+    <row r="50" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <f>SUM(Q46:Q49)</f>
+        <v>655360</v>
+      </c>
+    </row>
+    <row r="51" spans="14:17" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <f>P42-Q50</f>
+        <v>1690486</v>
       </c>
     </row>
   </sheetData>
@@ -1989,6 +2077,7 @@
     <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>